<commit_message>
merge with static map
</commit_message>
<xml_diff>
--- a/RICE13_pyomo/Results/coop.xlsx
+++ b/RICE13_pyomo/Results/coop.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="US" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="ES" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="EU" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="JAP" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="RUS" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="EUR" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="CHI" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="IND" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="MEST" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="AFR" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="LAM" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="OHI" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="OTH" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="global" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="US" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ES" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EU" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="JAP" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RUS" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EUR" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CHI" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="IND" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MEST" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AFR" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LAM" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OHI" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OTH" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="global" sheetId="14" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
added JSON func in --map scenrio
</commit_message>
<xml_diff>
--- a/RICE13_pyomo/Results/coop.xlsx
+++ b/RICE13_pyomo/Results/coop.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="US" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ES" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EU" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="JAP" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RUS" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EUR" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CHI" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="IND" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MEST" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AFR" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LAM" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OHI" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OTH" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="global" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="US" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="ES" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="EU" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="JAP" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="RUS" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="EUR" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="CHI" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="IND" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="MEST" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="AFR" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="LAM" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="OHI" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="OTH" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="global" sheetId="14" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>